<commit_message>
opt. separate the FileService and ExcelFileUtils
</commit_message>
<xml_diff>
--- a/src/main/resources/local/err.xlsx
+++ b/src/main/resources/local/err.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,12 +116,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>童子杰</t>
+          <t>俞鸿泰</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -138,20 +138,64 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>七七</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>牛马学院</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Connection refused: no further information: localhost/127.0.0.1:8081</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>童子杰</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>牛马学院</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Connection refused: no further information: localhost/127.0.0.1:8081</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>周云挺</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>牛马学院</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>牛马学院</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Connection refused: no further information: localhost/127.0.0.1:8081</t>
         </is>

</xml_diff>